<commit_message>
Hallo hier seht ihr eine tolle Beschreibung.
Ich habe GitHub geputzt.
</commit_message>
<xml_diff>
--- a/markdown/PackagesRProjekt.xlsx
+++ b/markdown/PackagesRProjekt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maren\Documents\GitHub\2022-topic-02-team-05\markdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255FB25D-BC71-4119-9D97-F0F6A6D70879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6822CB7A-EBC0-4CA6-9F97-8E7413DECFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CF1DC80D-AB90-D14E-9A8B-D78C95A1BD6C}"/>
+    <workbookView xWindow="3820" yWindow="1050" windowWidth="14400" windowHeight="7270" xr2:uid="{CF1DC80D-AB90-D14E-9A8B-D78C95A1BD6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>GSVA</t>
   </si>
   <si>
-    <t>ComplexHeatmap</t>
-  </si>
-  <si>
     <t>metaplot</t>
   </si>
   <si>
@@ -463,6 +460,9 @@
       </rPr>
       <t xml:space="preserve"> 2022</t>
     </r>
+  </si>
+  <si>
+    <t>Complex \ Heatmap</t>
   </si>
 </sst>
 </file>
@@ -833,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91197DA1-1283-2445-8AAE-77FFCAB9EC92}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -850,10 +850,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D1" s="1"/>
     </row>
@@ -862,10 +862,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -874,10 +874,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -886,10 +886,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -898,10 +898,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -910,10 +910,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -925,7 +925,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -937,7 +937,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -946,10 +946,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -958,142 +958,142 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="1"/>
     </row>

</xml_diff>